<commit_message>
added new way to carry out exams
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Secure-Online-Examination-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F35596A-B7FE-4122-A482-3D573BD32F8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69AF03A-B60A-43E0-BBA6-28856C129DF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="2175" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Matric</t>
-  </si>
-  <si>
     <t>hello</t>
   </si>
   <si>
@@ -46,6 +43,12 @@
   </si>
   <si>
     <t>nono@gm.com</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>aa@a.com</t>
   </si>
 </sst>
 </file>
@@ -374,51 +377,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>111</v>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>222</v>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{34DCA213-A807-4E2E-96D7-F83B94C36E90}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{E624EF04-5BB7-4CE8-9ECF-521406E4F590}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{A51407DF-B0D3-4DEF-8222-069583E7EFA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>